<commit_message>
update roanoke other revisions
</commit_message>
<xml_diff>
--- a/Cities-Counties-States.xlsx
+++ b/Cities-Counties-States.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mingchen/Desktop/Harvard/Courses/BST260/FinalProject/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A32B925-EAE8-8648-8344-3DB5A69107C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="工作表1" sheetId="1" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
   <si>
     <t>Location</t>
   </si>
@@ -446,55 +455,79 @@
   </si>
   <si>
     <t>TEXAS/NEW MEXICO</t>
+  </si>
+  <si>
+    <t>ROANOKE</t>
+  </si>
+  <si>
+    <t>STLOUIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="5"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -502,7 +535,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -512,56 +545,57 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -751,28 +785,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.86"/>
-    <col customWidth="1" min="2" max="2" width="16.14"/>
-    <col customWidth="1" min="3" max="3" width="19.14"/>
-    <col customWidth="1" min="4" max="4" width="15.71"/>
-    <col customWidth="1" min="5" max="5" width="34.86"/>
-    <col customWidth="1" min="6" max="6" width="21.43"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +851,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -825,10 +864,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -841,11 +880,11 @@
         <v>11</v>
       </c>
       <c r="F3" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -862,7 +901,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G4" s="7"/>
       <c r="I4" s="8"/>
@@ -884,7 +923,7 @@
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -897,11 +936,11 @@
         <v>18</v>
       </c>
       <c r="F5" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -914,11 +953,11 @@
         <v>21</v>
       </c>
       <c r="F6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -935,7 +974,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7"/>
       <c r="I7" s="8"/>
@@ -957,7 +996,7 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -968,11 +1007,11 @@
         <v>27</v>
       </c>
       <c r="F8" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -985,11 +1024,11 @@
         <v>30</v>
       </c>
       <c r="F9" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1002,11 +1041,11 @@
         <v>33</v>
       </c>
       <c r="F10" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1023,7 +1062,7 @@
         <v>38</v>
       </c>
       <c r="F11" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G11" s="7"/>
       <c r="I11" s="9"/>
@@ -1045,7 +1084,7 @@
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26">
       <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
@@ -1058,11 +1097,11 @@
         <v>38</v>
       </c>
       <c r="F12" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -1079,7 +1118,7 @@
         <v>45</v>
       </c>
       <c r="F13" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G13" s="7"/>
       <c r="I13" s="9"/>
@@ -1101,7 +1140,7 @@
       <c r="Y13" s="9"/>
       <c r="Z13" s="9"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26">
       <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
@@ -1114,11 +1153,11 @@
         <v>48</v>
       </c>
       <c r="F14" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26">
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
@@ -1131,11 +1170,11 @@
         <v>51</v>
       </c>
       <c r="F15" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -1148,11 +1187,11 @@
         <v>51</v>
       </c>
       <c r="F16" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26">
       <c r="A17" s="3" t="s">
         <v>54</v>
       </c>
@@ -1163,11 +1202,11 @@
         <v>51</v>
       </c>
       <c r="F17" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26">
       <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
@@ -1184,7 +1223,7 @@
         <v>59</v>
       </c>
       <c r="F18" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G18" s="7"/>
       <c r="I18" s="9"/>
@@ -1206,7 +1245,7 @@
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26">
       <c r="A19" s="3" t="s">
         <v>60</v>
       </c>
@@ -1223,7 +1262,7 @@
         <v>64</v>
       </c>
       <c r="F19" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="7"/>
       <c r="I19" s="9"/>
@@ -1245,7 +1284,7 @@
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26">
       <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1258,11 +1297,11 @@
         <v>45</v>
       </c>
       <c r="F20" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -1275,11 +1314,11 @@
         <v>69</v>
       </c>
       <c r="F21" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26">
       <c r="A22" s="3" t="s">
         <v>70</v>
       </c>
@@ -1292,11 +1331,11 @@
         <v>72</v>
       </c>
       <c r="F22" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26">
       <c r="A23" s="3" t="s">
         <v>73</v>
       </c>
@@ -1309,11 +1348,11 @@
         <v>75</v>
       </c>
       <c r="F23" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26">
       <c r="A24" s="3" t="s">
         <v>76</v>
       </c>
@@ -1326,11 +1365,11 @@
         <v>27</v>
       </c>
       <c r="F24" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26">
       <c r="A25" s="3" t="s">
         <v>78</v>
       </c>
@@ -1343,11 +1382,11 @@
         <v>80</v>
       </c>
       <c r="F25" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:26">
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>
@@ -1364,7 +1403,7 @@
         <v>72</v>
       </c>
       <c r="F26" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="7"/>
       <c r="I26" s="8"/>
@@ -1386,7 +1425,7 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:26">
       <c r="A27" s="3" t="s">
         <v>85</v>
       </c>
@@ -1397,11 +1436,11 @@
         <v>86</v>
       </c>
       <c r="F27" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:26">
       <c r="A28" s="3" t="s">
         <v>87</v>
       </c>
@@ -1414,11 +1453,11 @@
         <v>89</v>
       </c>
       <c r="F28" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:26">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -1435,11 +1474,11 @@
         <v>94</v>
       </c>
       <c r="F29" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26">
       <c r="A30" s="3" t="s">
         <v>95</v>
       </c>
@@ -1450,11 +1489,11 @@
         <v>8</v>
       </c>
       <c r="F30" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26">
       <c r="A31" s="3" t="s">
         <v>96</v>
       </c>
@@ -1465,11 +1504,11 @@
         <v>86</v>
       </c>
       <c r="F31" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:26">
       <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
@@ -1480,11 +1519,11 @@
         <v>86</v>
       </c>
       <c r="F32" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
         <v>98</v>
       </c>
@@ -1497,11 +1536,11 @@
         <v>72</v>
       </c>
       <c r="F33" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:7">
       <c r="A34" s="3" t="s">
         <v>100</v>
       </c>
@@ -1514,11 +1553,11 @@
         <v>59</v>
       </c>
       <c r="F34" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
         <v>102</v>
       </c>
@@ -1535,11 +1574,11 @@
         <v>106</v>
       </c>
       <c r="F35" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:7">
       <c r="A36" s="3" t="s">
         <v>107</v>
       </c>
@@ -1552,11 +1591,11 @@
         <v>59</v>
       </c>
       <c r="F36" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:7">
       <c r="A37" s="3" t="s">
         <v>109</v>
       </c>
@@ -1567,11 +1606,11 @@
         <v>86</v>
       </c>
       <c r="F37" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:7">
       <c r="A38" s="3" t="s">
         <v>110</v>
       </c>
@@ -1584,11 +1623,11 @@
         <v>112</v>
       </c>
       <c r="F38" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:7">
       <c r="A39" s="3" t="s">
         <v>113</v>
       </c>
@@ -1605,11 +1644,11 @@
         <v>30</v>
       </c>
       <c r="F39" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:7">
       <c r="A40" s="3" t="s">
         <v>116</v>
       </c>
@@ -1626,16 +1665,16 @@
         <v>118</v>
       </c>
       <c r="F40" s="4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:7">
       <c r="A41" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -1643,11 +1682,11 @@
         <v>118</v>
       </c>
       <c r="F41" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:7">
       <c r="A42" s="3" t="s">
         <v>120</v>
       </c>
@@ -1660,11 +1699,11 @@
         <v>27</v>
       </c>
       <c r="F42" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="7"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:7">
       <c r="A43" s="3" t="s">
         <v>122</v>
       </c>
@@ -1677,11 +1716,11 @@
         <v>27</v>
       </c>
       <c r="F43" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:7">
       <c r="A44" s="3" t="s">
         <v>124</v>
       </c>
@@ -1694,11 +1733,11 @@
         <v>27</v>
       </c>
       <c r="F44" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:7">
       <c r="A45" s="3" t="s">
         <v>126</v>
       </c>
@@ -1711,11 +1750,11 @@
         <v>128</v>
       </c>
       <c r="F45" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:7">
       <c r="A46" s="3" t="s">
         <v>129</v>
       </c>
@@ -1726,11 +1765,11 @@
         <v>130</v>
       </c>
       <c r="F46" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:7">
       <c r="A47" s="3" t="s">
         <v>131</v>
       </c>
@@ -1741,11 +1780,11 @@
         <v>86</v>
       </c>
       <c r="F47" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:7">
       <c r="A48" s="3" t="s">
         <v>132</v>
       </c>
@@ -1756,11 +1795,11 @@
         <v>86</v>
       </c>
       <c r="F48" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G48" s="7"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:7">
       <c r="A49" s="3" t="s">
         <v>133</v>
       </c>
@@ -1773,16 +1812,16 @@
         <v>128</v>
       </c>
       <c r="F49" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="7"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:7">
       <c r="A50" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -1790,11 +1829,11 @@
         <v>136</v>
       </c>
       <c r="F50" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="7"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:7">
       <c r="A51" s="3" t="s">
         <v>137</v>
       </c>
@@ -1807,11 +1846,11 @@
         <v>8</v>
       </c>
       <c r="F51" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="7"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:7">
       <c r="A52" s="3" t="s">
         <v>139</v>
       </c>
@@ -1824,11 +1863,11 @@
         <v>72</v>
       </c>
       <c r="F52" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:7">
       <c r="A53" s="3" t="s">
         <v>141</v>
       </c>
@@ -1839,11 +1878,11 @@
         <v>86</v>
       </c>
       <c r="F53" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G53" s="7"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:7">
       <c r="A54" s="3" t="s">
         <v>142</v>
       </c>
@@ -1854,11 +1893,11 @@
         <v>86</v>
       </c>
       <c r="F54" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G54" s="7"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:7">
       <c r="A55" s="3" t="s">
         <v>143</v>
       </c>
@@ -1869,14 +1908,15 @@
         <v>144</v>
       </c>
       <c r="F55" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G55" s="7"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:7">
       <c r="G56" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove stlouis and roanoke in data wrangling process
</commit_message>
<xml_diff>
--- a/Cities-Counties-States.xlsx
+++ b/Cities-Counties-States.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mingchen/Desktop/Harvard/Courses/BST260/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A32B925-EAE8-8648-8344-3DB5A69107C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1F27BE-1D60-A94A-AE91-100D2FE36F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -798,7 +798,7 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1682,7 +1682,7 @@
         <v>118</v>
       </c>
       <c r="F41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="7"/>
     </row>
@@ -1829,7 +1829,7 @@
         <v>136</v>
       </c>
       <c r="F50" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" s="7"/>
     </row>

</xml_diff>